<commit_message>
4gb file after running with output
</commit_message>
<xml_diff>
--- a/time_data.xlsx
+++ b/time_data.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+  <si>
+    <t>Data</t>
+  </si>
   <si>
     <t>500mb</t>
   </si>
@@ -1031,7 +1034,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.90780141843972" defaultRowHeight="12.7"/>
@@ -1049,51 +1052,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1243,17 +1248,17 @@
     </row>
     <row r="11" spans="8:8">
       <c r="H11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="6:6">
       <c r="F15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>